<commit_message>
getRooms function now expands abbreviated locations to buildings, floors, locations
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emiliobarreiro/Projects/MediaWorks Automated Requests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{963FEAFC-AF26-544D-BD4E-691CFAD5462C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BEE163A-A871-E649-9B60-C1234E0A2A78}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3320" yWindow="1980" windowWidth="23640" windowHeight="14420" activeTab="2" xr2:uid="{A9A68CCC-D4F4-1240-BC26-E578801BE1F1}"/>
+    <workbookView xWindow="2920" yWindow="1400" windowWidth="23640" windowHeight="14420" activeTab="2" xr2:uid="{A9A68CCC-D4F4-1240-BC26-E578801BE1F1}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="2" r:id="rId1"/>
     <sheet name="Equipment" sheetId="4" r:id="rId2"/>
-    <sheet name="Building Floor Room" sheetId="3" r:id="rId3"/>
+    <sheet name="Building Floor Room" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Name</t>
   </si>
@@ -41,36 +41,15 @@
     <t>Event</t>
   </si>
   <si>
-    <t>Odyssey of the Mind</t>
-  </si>
-  <si>
     <t>Start</t>
   </si>
   <si>
     <t>End</t>
   </si>
   <si>
-    <t>Building</t>
-  </si>
-  <si>
-    <t>CHASS INT NORTH</t>
-  </si>
-  <si>
-    <t>Floor</t>
-  </si>
-  <si>
-    <t>First Floor</t>
-  </si>
-  <si>
-    <t>Room</t>
-  </si>
-  <si>
     <t>FAU</t>
   </si>
   <si>
-    <t>A01405-19900-68</t>
-  </si>
-  <si>
     <t>Cost Center</t>
   </si>
   <si>
@@ -105,6 +84,87 @@
   </si>
   <si>
     <t>AFAPR</t>
+  </si>
+  <si>
+    <t>SKYE 171 </t>
+  </si>
+  <si>
+    <t>SKYE 172 </t>
+  </si>
+  <si>
+    <t>SKYE 173 </t>
+  </si>
+  <si>
+    <t>SPR 1102 </t>
+  </si>
+  <si>
+    <t>SPR 1340 </t>
+  </si>
+  <si>
+    <t>SPR 1358 </t>
+  </si>
+  <si>
+    <t>SPR 2212 </t>
+  </si>
+  <si>
+    <t>SPR 2339 </t>
+  </si>
+  <si>
+    <t>SPR 2340 </t>
+  </si>
+  <si>
+    <t>SPR 2343 </t>
+  </si>
+  <si>
+    <t>SPR 2344 </t>
+  </si>
+  <si>
+    <t>SPR 2351 </t>
+  </si>
+  <si>
+    <t>SPR 2355 </t>
+  </si>
+  <si>
+    <t>SPR 2356 </t>
+  </si>
+  <si>
+    <t>SPR 2360 </t>
+  </si>
+  <si>
+    <t>SPR 2361 </t>
+  </si>
+  <si>
+    <t>SPR 2364 </t>
+  </si>
+  <si>
+    <t>SPR 2365 </t>
+  </si>
+  <si>
+    <t>UNLH 1000 </t>
+  </si>
+  <si>
+    <t>WAT 1101 </t>
+  </si>
+  <si>
+    <t>WAT 1111 </t>
+  </si>
+  <si>
+    <t>WAT 1117 </t>
+  </si>
+  <si>
+    <t>WAT 2141 </t>
+  </si>
+  <si>
+    <t>WAT 2240</t>
+  </si>
+  <si>
+    <t>Locations</t>
+  </si>
+  <si>
+    <t>A02368-19900-68</t>
+  </si>
+  <si>
+    <t>AP Readiness</t>
   </si>
 </sst>
 </file>
@@ -131,7 +191,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="13"/>
+      <sz val="12"/>
       <color rgb="FF222222"/>
       <name val="Tahoma"/>
       <family val="2"/>
@@ -172,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -189,7 +249,11 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -507,7 +571,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -535,22 +599,22 @@
         <v>3</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>12</v>
-      </c>
       <c r="G1" s="4" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="H1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -561,25 +625,25 @@
         <v>9518271253</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="D2" s="3">
-        <v>0.33333333333333331</v>
+        <v>0.29166666666666669</v>
       </c>
       <c r="E2" s="3">
-        <v>0.70833333333333337</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="I2" s="5">
-        <v>43526</v>
+        <v>43554</v>
       </c>
     </row>
   </sheetData>
@@ -592,7 +656,7 @@
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -602,37 +666,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -641,241 +705,154 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70C9F1F1-01E0-3E4F-ACE4-67BFD9BBE0A4}">
-  <dimension ref="A1:E64"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5484D07-A62A-1342-8AF1-1A48E23A008B}">
+  <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="6"/>
-    </row>
-    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="2">
-        <v>1001</v>
-      </c>
-      <c r="E2" s="6"/>
-    </row>
-    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="2">
-        <v>1002</v>
-      </c>
-      <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E5" s="6"/>
-    </row>
-    <row r="6" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E6" s="6"/>
-    </row>
-    <row r="7" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E7" s="6"/>
-    </row>
-    <row r="8" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E10" s="6"/>
-    </row>
-    <row r="11" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E12" s="6"/>
-    </row>
-    <row r="13" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E13" s="6"/>
-    </row>
-    <row r="14" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E14" s="6"/>
-    </row>
-    <row r="15" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E15" s="6"/>
-    </row>
-    <row r="16" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E18" s="6"/>
-    </row>
-    <row r="19" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E19" s="6"/>
-    </row>
-    <row r="20" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E21" s="6"/>
-    </row>
-    <row r="22" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E22" s="6"/>
-    </row>
-    <row r="23" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E23" s="6"/>
-    </row>
-    <row r="24" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E24" s="6"/>
-    </row>
-    <row r="25" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E25" s="6"/>
-    </row>
-    <row r="26" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E26" s="6"/>
-    </row>
-    <row r="27" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E27" s="6"/>
-    </row>
-    <row r="28" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E28" s="6"/>
-    </row>
-    <row r="29" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E29" s="6"/>
-    </row>
-    <row r="30" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E30" s="6"/>
-    </row>
-    <row r="31" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E31" s="6"/>
-    </row>
-    <row r="32" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E32" s="6"/>
-    </row>
-    <row r="33" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E33" s="6"/>
-    </row>
-    <row r="34" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E34" s="6"/>
-    </row>
-    <row r="35" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E35" s="6"/>
-    </row>
-    <row r="36" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E36" s="6"/>
-    </row>
-    <row r="37" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E37" s="6"/>
-    </row>
-    <row r="38" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E38" s="6"/>
-    </row>
-    <row r="39" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E39" s="6"/>
-    </row>
-    <row r="40" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E40" s="6"/>
-    </row>
-    <row r="41" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E41" s="6"/>
-    </row>
-    <row r="42" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E42" s="6"/>
-    </row>
-    <row r="43" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E43" s="6"/>
-    </row>
-    <row r="44" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E44" s="6"/>
-    </row>
-    <row r="45" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E45" s="6"/>
-    </row>
-    <row r="46" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E46" s="6"/>
-    </row>
-    <row r="47" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E47" s="6"/>
-    </row>
-    <row r="48" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E48" s="6"/>
-    </row>
-    <row r="49" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E49" s="6"/>
-    </row>
-    <row r="50" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E50" s="6"/>
-    </row>
-    <row r="51" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E51" s="6"/>
-    </row>
-    <row r="52" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E52" s="6"/>
-    </row>
-    <row r="53" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E53" s="6"/>
-    </row>
-    <row r="54" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E54" s="6"/>
-    </row>
-    <row r="55" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E55" s="6"/>
-    </row>
-    <row r="56" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E56" s="6"/>
-    </row>
-    <row r="57" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E57" s="6"/>
-    </row>
-    <row r="58" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E58" s="6"/>
-    </row>
-    <row r="59" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E59" s="6"/>
-    </row>
-    <row r="60" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E60" s="6"/>
-    </row>
-    <row r="61" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E61" s="6"/>
-    </row>
-    <row r="62" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E62" s="6"/>
-    </row>
-    <row r="63" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E63" s="6"/>
-    </row>
-    <row r="64" spans="5:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="E64" s="6"/>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="7"/>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="7"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="7"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="7"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>